<commit_message>
break neighbourhood symettries, about to set small iterations to investigate
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TravelOptimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C7ED45-3625-F14E-BBEA-D4A016A23D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A5C24F-3C60-C64B-90C3-7B172022C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
+    <workbookView xWindow="12280" yWindow="680" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
   <sheets>
     <sheet name="04 Sep" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -165,37 +165,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -218,11 +188,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -539,7 +509,7 @@
   <dimension ref="B4:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -686,7 +656,7 @@
         <v>36.020000000000003</v>
       </c>
       <c r="E10">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F10">
         <v>195</v>
@@ -696,7 +666,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -956,7 +926,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="E22">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="F22">
         <v>325</v>
@@ -966,18 +936,18 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>-52</v>
+        <v>-36</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="J6:J22">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
parse_solution.py works well for a file path now, remove redundant files
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TravelOptimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39A5C24F-3C60-C64B-90C3-7B172022C9D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5D7A1F-2C1B-BF4C-AEBC-20E631B93D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12280" yWindow="680" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
   <sheets>
     <sheet name="04 Sep" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add a stagnation threshold for SLS, make it 2n, back to 3 neighbourhoods, achieve great results for CON12
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TravelOptimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5D7A1F-2C1B-BF4C-AEBC-20E631B93D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06B1D755-B407-2A41-B92A-D02F8E7347B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
   <sheets>
     <sheet name="04 Sep" sheetId="1" r:id="rId1"/>
@@ -608,7 +608,7 @@
         <v>7.6</v>
       </c>
       <c r="E8">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8">
         <v>84</v>
@@ -618,7 +618,7 @@
       </c>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.2">
@@ -632,7 +632,7 @@
         <v>13.55</v>
       </c>
       <c r="E9">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="F9">
         <v>134</v>
@@ -642,7 +642,7 @@
       </c>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>-7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
@@ -656,7 +656,7 @@
         <v>36.020000000000003</v>
       </c>
       <c r="E10">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="F10">
         <v>195</v>
@@ -666,7 +666,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>46.01</v>
       </c>
       <c r="E11">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="F11">
         <v>275</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-19</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -704,7 +704,7 @@
         <v>10.76</v>
       </c>
       <c r="E12">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F12">
         <v>361</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>-18</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -773,14 +773,14 @@
         <v>6.46</v>
       </c>
       <c r="E15">
-        <v>44245</v>
+        <v>42211</v>
       </c>
       <c r="G15">
         <v>41505</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>-2740</v>
+        <v>-706</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">
@@ -794,14 +794,14 @@
         <v>2.68</v>
       </c>
       <c r="E16">
-        <v>71452</v>
+        <v>70237</v>
       </c>
       <c r="G16">
         <v>60293</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>-11159</v>
+        <v>-9944</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -815,14 +815,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E17">
-        <v>137474</v>
+        <v>133682</v>
       </c>
       <c r="G17">
         <v>120696</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>-16778</v>
+        <v>-12986</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -836,14 +836,14 @@
         <v>8.42</v>
       </c>
       <c r="E18">
-        <v>262761</v>
+        <v>247736</v>
       </c>
       <c r="G18">
         <v>207343</v>
       </c>
       <c r="J18">
         <f t="shared" si="0"/>
-        <v>-55418</v>
+        <v>-40393</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
@@ -857,14 +857,14 @@
         <v>11.27</v>
       </c>
       <c r="E19">
-        <v>367311</v>
+        <v>350399</v>
       </c>
       <c r="G19">
         <v>285614</v>
       </c>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>-81697</v>
+        <v>-64785</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>2.93</v>
       </c>
       <c r="E20">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F20">
         <v>72</v>
@@ -888,7 +888,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="E22">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="F22">
         <v>325</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>-36</v>
+        <v>-30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
classify instance files for better inspection
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TravelOptimization/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TTP_solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB1AB34-36EB-9546-B8CA-D06471F5F6AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F491B5B-D5BB-4B40-B45A-6BA2BEA08740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="B4:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -656,7 +656,7 @@
         <v>36.020000000000003</v>
       </c>
       <c r="E10">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F10">
         <v>195</v>
@@ -666,7 +666,7 @@
       </c>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
@@ -680,7 +680,7 @@
         <v>46.01</v>
       </c>
       <c r="E11">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F11">
         <v>275</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -704,7 +704,7 @@
         <v>10.76</v>
       </c>
       <c r="E12">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="F12">
         <v>361</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -878,7 +878,7 @@
         <v>2.93</v>
       </c>
       <c r="E20">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F20">
         <v>72</v>
@@ -888,7 +888,7 @@
       </c>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="E22">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="F22">
         <v>325</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>-30</v>
+        <v>-24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalising the idea of VNS and tabu, with some more results
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TTP_solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F491B5B-D5BB-4B40-B45A-6BA2BEA08740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548AB9E-45AF-694D-A216-408368F9B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="B4:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -704,7 +704,7 @@
         <v>10.76</v>
       </c>
       <c r="E12">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="F12">
         <v>361</v>
@@ -714,7 +714,7 @@
       </c>
       <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.2">
@@ -794,14 +794,14 @@
         <v>2.68</v>
       </c>
       <c r="E16">
-        <v>70237</v>
+        <v>65401</v>
       </c>
       <c r="G16">
         <v>60293</v>
       </c>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>-9944</v>
+        <v>-5108</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
@@ -815,14 +815,14 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="E17">
-        <v>133682</v>
+        <v>129269</v>
       </c>
       <c r="G17">
         <v>120696</v>
       </c>
       <c r="J17">
         <f t="shared" si="0"/>
-        <v>-12986</v>
+        <v>-8573</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
@@ -902,7 +902,7 @@
         <v>1.1299999999999999</v>
       </c>
       <c r="E21">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F21">
         <v>160</v>
@@ -912,7 +912,7 @@
       </c>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>-16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
@@ -926,7 +926,7 @@
         <v>2.4300000000000002</v>
       </c>
       <c r="E22">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="F22">
         <v>325</v>
@@ -936,7 +936,7 @@
       </c>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>-24</v>
+        <v>-12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refine tabu list logic, get the connecting neighbourhood for NL6 optimal, create dfs_star scaffold
</commit_message>
<xml_diff>
--- a/TTP result.xlsx
+++ b/TTP result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/2716162381qq.com/Desktop/TTP_solver/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4548AB9E-45AF-694D-A216-408368F9B591}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DFF35DE-F292-774B-9B0E-35B94349FCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{79B9E0B9-42A9-EB45-B883-2D26E5C835F4}"/>
   </bookViews>
@@ -509,7 +509,7 @@
   <dimension ref="B4:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -680,7 +680,7 @@
         <v>46.01</v>
       </c>
       <c r="E11">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F11">
         <v>275</v>
@@ -690,7 +690,7 @@
       </c>
       <c r="J11">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
@@ -773,14 +773,14 @@
         <v>6.46</v>
       </c>
       <c r="E15">
-        <v>42211</v>
+        <v>41959</v>
       </c>
       <c r="G15">
         <v>41505</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>-706</v>
+        <v>-454</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.2">

</xml_diff>